<commit_message>
Changed input data and documentation of deterministic model
</commit_message>
<xml_diff>
--- a/Input_clsp.xlsx
+++ b/Input_clsp.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fredericweiss/Documents/Repositories/Lot-Sizing-Problem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296C04CC-9D46-E24D-9802-DBC9A4808778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93E55C4-4068-B74D-85B4-163785923402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{80E0BF24-455B-B347-860D-91671CA7ADCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEED4FD-B98A-2E41-ABE4-8902EF5A0B8F}">
   <dimension ref="B2:AU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +458,8 @@
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="8" max="47" width="4.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="47" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
@@ -615,124 +616,124 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>556</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>526</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>516</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>481</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>532</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="S3">
-        <v>247</v>
+        <v>309</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="U3">
-        <v>321</v>
+        <v>208</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>590</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>257</v>
       </c>
       <c r="Z3">
-        <v>484</v>
+        <v>412</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>378</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>498</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>592</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>583</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>214</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>541</v>
       </c>
       <c r="AK3">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="AL3">
-        <v>750</v>
+        <v>14</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="AN3">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="AO3">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AQ3">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="AR3">
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="AS3">
-        <v>0</v>
+        <v>431</v>
       </c>
       <c r="AT3">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="AU3">
-        <v>0</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="2:47" x14ac:dyDescent="0.2">
@@ -752,124 +753,124 @@
         <v>5</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>274</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>199</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="M4">
-        <v>807</v>
+        <v>228</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>572</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="U4">
-        <v>906</v>
+        <v>533</v>
       </c>
       <c r="V4">
-        <v>722</v>
+        <v>553</v>
       </c>
       <c r="W4">
-        <v>309</v>
+        <v>136</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AA4">
-        <v>142</v>
+        <v>195</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="AC4">
-        <v>450</v>
+        <v>399</v>
       </c>
       <c r="AD4">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <v>542</v>
       </c>
       <c r="AF4">
-        <v>0</v>
+        <v>266</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>266</v>
       </c>
       <c r="AH4">
-        <v>0</v>
+        <v>548</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="AK4">
-        <v>0</v>
+        <v>413</v>
       </c>
       <c r="AL4">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>545</v>
       </c>
       <c r="AN4">
-        <v>0</v>
+        <v>453</v>
       </c>
       <c r="AO4">
-        <v>0</v>
+        <v>442</v>
       </c>
       <c r="AP4">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="AQ4">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="AR4">
-        <v>0</v>
+        <v>493</v>
       </c>
       <c r="AS4">
-        <v>0</v>
+        <v>492</v>
       </c>
       <c r="AT4">
-        <v>12</v>
+        <v>458</v>
       </c>
       <c r="AU4">
-        <v>0</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="2:47" x14ac:dyDescent="0.2">
@@ -889,124 +890,124 @@
         <v>6</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>587</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="L5">
-        <v>346</v>
+        <v>386</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="N5">
-        <v>653</v>
+        <v>504</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="P5">
-        <v>747</v>
+        <v>291</v>
       </c>
       <c r="Q5">
-        <v>811</v>
+        <v>28</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>216</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="V5">
-        <v>636</v>
+        <v>305</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>482</v>
       </c>
       <c r="Z5">
-        <v>348</v>
+        <v>221</v>
       </c>
       <c r="AA5">
-        <v>370</v>
+        <v>62</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="AC5">
         <v>0</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AG5">
-        <v>238</v>
+        <v>395</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>521</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>358</v>
       </c>
       <c r="AK5">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="AL5">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="AM5">
         <v>0</v>
       </c>
       <c r="AN5">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="AO5">
-        <v>0</v>
+        <v>576</v>
       </c>
       <c r="AP5">
-        <v>0</v>
+        <v>445</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="AR5">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="AS5">
-        <v>550</v>
+        <v>445</v>
       </c>
       <c r="AT5">
         <v>0</v>
       </c>
       <c r="AU5">
-        <v>0</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="2:47" x14ac:dyDescent="0.2">
@@ -1026,121 +1027,121 @@
         <v>7</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="M6">
-        <v>325</v>
+        <v>288</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
+        <v>187</v>
+      </c>
+      <c r="R6">
+        <v>52</v>
+      </c>
+      <c r="S6">
+        <v>105</v>
+      </c>
+      <c r="T6">
+        <v>175</v>
+      </c>
+      <c r="U6">
+        <v>67</v>
+      </c>
+      <c r="V6">
+        <v>62</v>
+      </c>
+      <c r="W6">
+        <v>328</v>
+      </c>
+      <c r="X6">
+        <v>31</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>334</v>
+      </c>
+      <c r="AA6">
+        <v>382</v>
+      </c>
+      <c r="AB6">
+        <v>71</v>
+      </c>
+      <c r="AC6">
+        <v>313</v>
+      </c>
+      <c r="AD6">
+        <v>57</v>
+      </c>
+      <c r="AE6">
+        <v>118</v>
+      </c>
+      <c r="AF6">
+        <v>34</v>
+      </c>
+      <c r="AG6">
+        <v>589</v>
+      </c>
+      <c r="AH6">
+        <v>80</v>
+      </c>
+      <c r="AI6">
+        <v>460</v>
+      </c>
+      <c r="AJ6">
+        <v>375</v>
+      </c>
+      <c r="AK6">
         <v>60</v>
       </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>354</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>877</v>
-      </c>
-      <c r="AI6">
-        <v>735</v>
-      </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>115</v>
-      </c>
       <c r="AL6">
-        <v>880</v>
+        <v>0</v>
       </c>
       <c r="AM6">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="AN6">
         <v>0</v>
       </c>
       <c r="AO6">
-        <v>0</v>
+        <v>461</v>
       </c>
       <c r="AP6">
-        <v>0</v>
+        <v>296</v>
       </c>
       <c r="AQ6">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="AR6">
-        <v>0</v>
+        <v>237</v>
       </c>
       <c r="AS6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AT6">
-        <v>0</v>
+        <v>552</v>
       </c>
       <c r="AU6">
         <v>0</v>
@@ -1163,82 +1164,82 @@
         <v>8</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>224</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>331</v>
       </c>
       <c r="L7">
-        <v>821</v>
+        <v>483</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>506</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>387</v>
       </c>
       <c r="O7">
-        <v>197</v>
+        <v>97</v>
       </c>
       <c r="P7">
-        <v>704</v>
+        <v>387</v>
       </c>
       <c r="Q7">
-        <v>486</v>
+        <v>113</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>570</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="T7">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>318</v>
       </c>
       <c r="V7">
-        <v>479</v>
+        <v>171</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <v>414</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="AA7">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <v>419</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>341</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <v>378</v>
       </c>
       <c r="AE7">
-        <v>365</v>
+        <v>99</v>
       </c>
       <c r="AF7">
-        <v>0</v>
+        <v>216</v>
       </c>
       <c r="AG7">
-        <v>854</v>
+        <v>35</v>
       </c>
       <c r="AH7">
         <v>0</v>
@@ -1247,40 +1248,40 @@
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="AK7">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="AL7">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="AN7">
-        <v>119</v>
+        <v>518</v>
       </c>
       <c r="AO7">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="AP7">
-        <v>116</v>
+        <v>579</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="AR7">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="AS7">
-        <v>842</v>
+        <v>0</v>
       </c>
       <c r="AT7">
-        <v>0</v>
+        <v>454</v>
       </c>
       <c r="AU7">
-        <v>804</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="2:47" x14ac:dyDescent="0.2">
@@ -1300,124 +1301,124 @@
         <v>9</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>536</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="N8">
-        <v>841</v>
+        <v>235</v>
       </c>
       <c r="O8">
-        <v>928</v>
+        <v>81</v>
       </c>
       <c r="P8">
-        <v>205</v>
+        <v>449</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>487</v>
       </c>
       <c r="R8">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="S8">
-        <v>562</v>
+        <v>219</v>
       </c>
       <c r="T8">
-        <v>56</v>
+        <v>340</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W8">
-        <v>769</v>
+        <v>496</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="AB8">
-        <v>1800</v>
+        <v>81</v>
       </c>
       <c r="AC8">
+        <v>378</v>
+      </c>
+      <c r="AD8">
+        <v>259</v>
+      </c>
+      <c r="AE8">
+        <v>319</v>
+      </c>
+      <c r="AF8">
+        <v>578</v>
+      </c>
+      <c r="AG8">
+        <v>310</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>462</v>
+      </c>
+      <c r="AJ8">
         <v>12</v>
       </c>
-      <c r="AD8">
-        <v>221</v>
-      </c>
-      <c r="AE8">
-        <v>469</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
       <c r="AK8">
-        <v>0</v>
+        <v>598</v>
       </c>
       <c r="AL8">
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="AM8">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="AN8">
-        <v>0</v>
+        <v>414</v>
       </c>
       <c r="AO8">
         <v>0</v>
       </c>
       <c r="AP8">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="AQ8">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="AR8">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="AS8">
-        <v>0</v>
+        <v>229</v>
       </c>
       <c r="AT8">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="AU8">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:47" x14ac:dyDescent="0.2">
@@ -1437,124 +1438,124 @@
         <v>10</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>521</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>523</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>505</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>432</v>
       </c>
       <c r="O9">
-        <v>10</v>
+        <v>553</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="Q9">
-        <v>22</v>
+        <v>292</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>553</v>
       </c>
       <c r="S9">
-        <v>522</v>
+        <v>333</v>
       </c>
       <c r="T9">
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>545</v>
       </c>
       <c r="V9">
-        <v>880</v>
+        <v>193</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>374</v>
       </c>
       <c r="AA9">
-        <v>612</v>
+        <v>556</v>
       </c>
       <c r="AB9">
-        <v>801</v>
+        <v>235</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="AE9">
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="AH9">
-        <v>452</v>
+        <v>310</v>
       </c>
       <c r="AI9">
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="AJ9">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="AK9">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="AL9">
-        <v>0</v>
+        <v>591</v>
       </c>
       <c r="AM9">
-        <v>0</v>
+        <v>552</v>
       </c>
       <c r="AN9">
-        <v>0</v>
+        <v>479</v>
       </c>
       <c r="AO9">
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="AP9">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="AQ9">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="AR9">
-        <v>974</v>
+        <v>15</v>
       </c>
       <c r="AS9">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="AT9">
-        <v>0</v>
+        <v>282</v>
       </c>
       <c r="AU9">
-        <v>0</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="2:47" x14ac:dyDescent="0.2">
@@ -1562,7 +1563,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>1000</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>